<commit_message>
feat: refactor db queries
</commit_message>
<xml_diff>
--- a/template/commercial-offer.xlsx
+++ b/template/commercial-offer.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\zfp-fans-backend\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C344F78-0CF4-43DE-BAF9-6C99E9750D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E8D043-6F62-4562-9F43-00A56CE77A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТКП" sheetId="2" r:id="rId1"/>
-    <sheet name="Шаблон" sheetId="3" r:id="rId2"/>
+    <sheet name="Подвал" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ТКП!$A$1:$P$2897</definedName>
@@ -1554,7 +1554,7 @@
       <c r="B11" s="14"/>
       <c r="C11" s="92">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45332</v>
       </c>
       <c r="D11" s="92"/>
       <c r="E11" s="92"/>

</xml_diff>

<commit_message>
feat: remove 1,9 model and fix regexp for bold text, update template
</commit_message>
<xml_diff>
--- a/template/commercial-offer.xlsx
+++ b/template/commercial-offer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\zfp-fans-backend\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E8D043-6F62-4562-9F43-00A56CE77A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E37FD2-3E77-4429-861F-A2B620B0EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="22308" windowHeight="11532" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТКП" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ТКП!$A$1:$P$2897</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -83,25 +83,13 @@
     <t>Итого со скидкой, Евро</t>
   </si>
   <si>
-    <t>Цена за шт. розница, USD</t>
-  </si>
-  <si>
     <t>Цена за шт. розница, Рубли</t>
-  </si>
-  <si>
-    <t>Цена за шт. со скидкой, USD</t>
   </si>
   <si>
     <t>Цена за шт. со скидкой, Рубли</t>
   </si>
   <si>
-    <t>Итого со скидкой, USD</t>
-  </si>
-  <si>
     <t>Итого со скидкой, Рубли</t>
-  </si>
-  <si>
-    <t>USD:</t>
   </si>
   <si>
     <t>Рубли:</t>
@@ -142,6 +130,18 @@
   </si>
   <si>
     <t>ТЕХНИКО-КОММЕРЧЕСКОЕ ПРЕДЛОЖЕНИЕ № 21-0000</t>
+  </si>
+  <si>
+    <t>CNY:</t>
+  </si>
+  <si>
+    <t>Цена за шт. розница, CNY</t>
+  </si>
+  <si>
+    <t>Цена за шт. со скидкой, CNY</t>
+  </si>
+  <si>
+    <t>Итого со скидкой, CNY</t>
   </si>
 </sst>
 </file>
@@ -1013,37 +1013,54 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>952499</xdr:colOff>
+      <xdr:colOff>8832</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>15162</xdr:rowOff>
+      <xdr:rowOff>52898</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
+        <xdr:cNvPr id="5" name="Рисунок 4" descr="C:\Users\kmuhin\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\5MAB4E1J\2024_BREEZ_price_shapka (002).jpg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10651E18-F26D-46B1-BD86-16F4CAEAF925}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="15687674" cy="1691562"/>
+          <a:ext cx="15222855" cy="1680807"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1401,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2897"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="88" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I2413" sqref="I2413"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="88" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1554,7 +1571,7 @@
       <c r="B11" s="14"/>
       <c r="C11" s="92">
         <f ca="1">TODAY()</f>
-        <v>45332</v>
+        <v>45581</v>
       </c>
       <c r="D11" s="92"/>
       <c r="E11" s="92"/>
@@ -1590,7 +1607,7 @@
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="90"/>
       <c r="C13" s="90"/>
@@ -1814,10 +1831,10 @@
         <v>16</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I24" s="26" t="s">
         <v>9</v>
@@ -1826,10 +1843,10 @@
         <v>17</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M24" s="27" t="s">
         <v>10</v>
@@ -1838,10 +1855,10 @@
         <v>18</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="P24" s="62" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -56458,7 +56475,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -56481,10 +56498,10 @@
         <v>11</v>
       </c>
       <c r="O1" s="45" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -56537,7 +56554,7 @@
     <row r="4" spans="1:16" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63"/>
       <c r="B4" s="97" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="98"/>
       <c r="D4" s="98"/>
@@ -56573,7 +56590,7 @@
       <c r="K5" s="56"/>
       <c r="L5" s="57"/>
       <c r="M5" s="33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N5" s="34" t="e">
         <f>O2</f>
@@ -56596,7 +56613,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="38"/>
       <c r="M6" s="35" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N6" s="36" t="e">
         <f>P2</f>
@@ -56607,7 +56624,7 @@
     </row>
     <row r="7" spans="1:16" s="12" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="106" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" s="107"/>
       <c r="C7" s="107"/>

</xml_diff>

<commit_message>
feat: upd template header and version
</commit_message>
<xml_diff>
--- a/template/commercial-offer.xlsx
+++ b/template/commercial-offer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\zfp-fans-backend\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E37FD2-3E77-4429-861F-A2B620B0EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BA2C74-8493-43D9-97F8-C9974A1599D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="0" windowWidth="22308" windowHeight="11532" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТКП" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ТКП!$A$1:$P$2897</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -1013,7 +1013,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>8832</xdr:colOff>
+      <xdr:colOff>978477</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>52898</xdr:rowOff>
     </xdr:to>
@@ -1046,7 +1046,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="15222855" cy="1680807"/>
+          <a:ext cx="16192500" cy="1680807"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2897"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="88" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="88" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1571,7 +1571,7 @@
       <c r="B11" s="14"/>
       <c r="C11" s="92">
         <f ca="1">TODAY()</f>
-        <v>45581</v>
+        <v>45582</v>
       </c>
       <c r="D11" s="92"/>
       <c r="E11" s="92"/>

</xml_diff>